<commit_message>
ngoc moi cap nhat
</commit_message>
<xml_diff>
--- a/KẾ HOẠCH CHI TIẾT.xlsx
+++ b/KẾ HOẠCH CHI TIẾT.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dowload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub\cay-nhi-phan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C4D3DB-0723-45BA-A8B1-01E34D9A564B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACFF76F-EEE3-44E5-8F3D-5BCDED881E39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4065" xr2:uid="{AFE64996-C6F0-4364-80A5-09C90EDB035F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual" concurrentCalc="0"/>
+  <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>KẾ HOẠCH &amp; PHÂN CÔNG LÀM ĐỒ ÁN MÔN CẤU TRÚC DỮ LIỆU VÀ GIẢI THUẬT</t>
   </si>
@@ -246,7 +246,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -256,7 +256,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -601,7 +600,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,57 +608,57 @@
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="7" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="17" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17" t="s">
+      <c r="E3" s="15"/>
+      <c r="F3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="16"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
@@ -669,8 +668,10 @@
       <c r="D4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="9" t="s">
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="3" t="s">

</xml_diff>